<commit_message>
added new features based off meeting
</commit_message>
<xml_diff>
--- a/server/data/TestSubset.xlsx
+++ b/server/data/TestSubset.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayden\Coding Projects\ForestryOnlineDatabase\server\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF15E7DB-FEF2-4485-941A-EE584180747C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23873D4-D016-4A8C-8528-586ED2E5665C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AN$35</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -881,17 +884,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1230,18 +1233,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN36"/>
+  <dimension ref="A1:AN35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K11"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="11" max="11" width="9.9140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="16" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1363,20 +1366,20 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:40" ht="16" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.4">
       <c r="A2" s="21">
         <v>202</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="24" t="s">
         <v>36</v>
       </c>
       <c r="F2" s="20" t="s">
@@ -1394,58 +1397,58 @@
       <c r="J2" s="20">
         <v>1</v>
       </c>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23" t="s">
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="23" t="s">
+      <c r="P2" s="24" t="s">
         <v>56</v>
       </c>
       <c r="Q2" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="R2" s="25" t="s">
+      <c r="R2" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="S2" s="26"/>
-      <c r="T2" s="25" t="s">
+      <c r="S2" s="25"/>
+      <c r="T2" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="U2" s="25" t="s">
+      <c r="U2" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="V2" s="25" t="s">
+      <c r="V2" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="W2" s="25"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="25"/>
-      <c r="Z2" s="25"/>
-      <c r="AA2" s="25"/>
-      <c r="AB2" s="25"/>
-      <c r="AC2" s="25"/>
-      <c r="AD2" s="23" t="s">
+      <c r="W2" s="26"/>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="26"/>
+      <c r="Z2" s="26"/>
+      <c r="AA2" s="26"/>
+      <c r="AB2" s="26"/>
+      <c r="AC2" s="26"/>
+      <c r="AD2" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="AE2" s="23" t="s">
+      <c r="AE2" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="AF2" s="23" t="s">
+      <c r="AF2" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="AG2" s="23" t="s">
+      <c r="AG2" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="AH2" s="23" t="s">
+      <c r="AH2" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="AI2" s="23" t="s">
+      <c r="AI2" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="AJ2" s="27"/>
+      <c r="AJ2" s="29"/>
       <c r="AK2" s="20" t="s">
         <v>72</v>
       </c>
@@ -1459,403 +1462,403 @@
         <v>-122.48609329999999</v>
       </c>
     </row>
-    <row r="3" spans="1:40" ht="16" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.4">
       <c r="A3" s="21"/>
       <c r="B3" s="22"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
       <c r="Q3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="R3" s="25"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="25"/>
-      <c r="V3" s="25"/>
-      <c r="W3" s="25"/>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
-      <c r="AA3" s="25"/>
-      <c r="AB3" s="25"/>
-      <c r="AC3" s="25"/>
-      <c r="AD3" s="23"/>
-      <c r="AE3" s="23"/>
-      <c r="AF3" s="23"/>
-      <c r="AG3" s="23"/>
-      <c r="AH3" s="23"/>
-      <c r="AI3" s="23"/>
-      <c r="AJ3" s="27"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="26"/>
+      <c r="U3" s="26"/>
+      <c r="V3" s="26"/>
+      <c r="W3" s="26"/>
+      <c r="X3" s="26"/>
+      <c r="Y3" s="26"/>
+      <c r="Z3" s="26"/>
+      <c r="AA3" s="26"/>
+      <c r="AB3" s="26"/>
+      <c r="AC3" s="26"/>
+      <c r="AD3" s="24"/>
+      <c r="AE3" s="24"/>
+      <c r="AF3" s="24"/>
+      <c r="AG3" s="24"/>
+      <c r="AH3" s="24"/>
+      <c r="AI3" s="24"/>
+      <c r="AJ3" s="29"/>
       <c r="AK3" s="20"/>
       <c r="AL3" s="20"/>
       <c r="AM3" s="20"/>
       <c r="AN3" s="20"/>
     </row>
-    <row r="4" spans="1:40" ht="16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.4">
       <c r="A4" s="21"/>
       <c r="B4" s="22"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
       <c r="Q4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="R4" s="25"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="25"/>
-      <c r="V4" s="25"/>
-      <c r="W4" s="25"/>
-      <c r="X4" s="25"/>
-      <c r="Y4" s="25"/>
-      <c r="Z4" s="25"/>
-      <c r="AA4" s="25"/>
-      <c r="AB4" s="25"/>
-      <c r="AC4" s="25"/>
-      <c r="AD4" s="23"/>
-      <c r="AE4" s="23"/>
-      <c r="AF4" s="23"/>
-      <c r="AG4" s="23"/>
-      <c r="AH4" s="23"/>
-      <c r="AI4" s="23"/>
-      <c r="AJ4" s="27"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="26"/>
+      <c r="V4" s="26"/>
+      <c r="W4" s="26"/>
+      <c r="X4" s="26"/>
+      <c r="Y4" s="26"/>
+      <c r="Z4" s="26"/>
+      <c r="AA4" s="26"/>
+      <c r="AB4" s="26"/>
+      <c r="AC4" s="26"/>
+      <c r="AD4" s="24"/>
+      <c r="AE4" s="24"/>
+      <c r="AF4" s="24"/>
+      <c r="AG4" s="24"/>
+      <c r="AH4" s="24"/>
+      <c r="AI4" s="24"/>
+      <c r="AJ4" s="29"/>
       <c r="AK4" s="20"/>
       <c r="AL4" s="20"/>
       <c r="AM4" s="20"/>
       <c r="AN4" s="20"/>
     </row>
-    <row r="5" spans="1:40" ht="16" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.4">
       <c r="A5" s="21"/>
       <c r="B5" s="22"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
       <c r="Q5" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="R5" s="25"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="25"/>
-      <c r="V5" s="25"/>
-      <c r="W5" s="25"/>
-      <c r="X5" s="25"/>
-      <c r="Y5" s="25"/>
-      <c r="Z5" s="25"/>
-      <c r="AA5" s="25"/>
-      <c r="AB5" s="25"/>
-      <c r="AC5" s="25"/>
-      <c r="AD5" s="23"/>
-      <c r="AE5" s="23"/>
-      <c r="AF5" s="23"/>
-      <c r="AG5" s="23"/>
-      <c r="AH5" s="23"/>
-      <c r="AI5" s="23"/>
-      <c r="AJ5" s="27"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="26"/>
+      <c r="X5" s="26"/>
+      <c r="Y5" s="26"/>
+      <c r="Z5" s="26"/>
+      <c r="AA5" s="26"/>
+      <c r="AB5" s="26"/>
+      <c r="AC5" s="26"/>
+      <c r="AD5" s="24"/>
+      <c r="AE5" s="24"/>
+      <c r="AF5" s="24"/>
+      <c r="AG5" s="24"/>
+      <c r="AH5" s="24"/>
+      <c r="AI5" s="24"/>
+      <c r="AJ5" s="29"/>
       <c r="AK5" s="20"/>
       <c r="AL5" s="20"/>
       <c r="AM5" s="20"/>
       <c r="AN5" s="20"/>
     </row>
-    <row r="6" spans="1:40" ht="16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.4">
       <c r="A6" s="21"/>
       <c r="B6" s="22"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
       <c r="H6" s="20"/>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
       <c r="Q6" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="R6" s="25"/>
-      <c r="S6" s="26"/>
-      <c r="T6" s="25"/>
-      <c r="U6" s="25"/>
-      <c r="V6" s="25"/>
-      <c r="W6" s="25"/>
-      <c r="X6" s="25"/>
-      <c r="Y6" s="25"/>
-      <c r="Z6" s="25"/>
-      <c r="AA6" s="25"/>
-      <c r="AB6" s="25"/>
-      <c r="AC6" s="25"/>
-      <c r="AD6" s="23"/>
-      <c r="AE6" s="23"/>
-      <c r="AF6" s="23"/>
-      <c r="AG6" s="23"/>
-      <c r="AH6" s="23"/>
-      <c r="AI6" s="23"/>
-      <c r="AJ6" s="27"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="26"/>
+      <c r="W6" s="26"/>
+      <c r="X6" s="26"/>
+      <c r="Y6" s="26"/>
+      <c r="Z6" s="26"/>
+      <c r="AA6" s="26"/>
+      <c r="AB6" s="26"/>
+      <c r="AC6" s="26"/>
+      <c r="AD6" s="24"/>
+      <c r="AE6" s="24"/>
+      <c r="AF6" s="24"/>
+      <c r="AG6" s="24"/>
+      <c r="AH6" s="24"/>
+      <c r="AI6" s="24"/>
+      <c r="AJ6" s="29"/>
       <c r="AK6" s="20"/>
       <c r="AL6" s="20"/>
       <c r="AM6" s="20"/>
       <c r="AN6" s="20"/>
     </row>
-    <row r="7" spans="1:40" ht="16" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.4">
       <c r="A7" s="21"/>
       <c r="B7" s="22"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
       <c r="I7" s="20"/>
       <c r="J7" s="20"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
       <c r="Q7" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="R7" s="25"/>
-      <c r="S7" s="26"/>
-      <c r="T7" s="25"/>
-      <c r="U7" s="25"/>
-      <c r="V7" s="25"/>
-      <c r="W7" s="25"/>
-      <c r="X7" s="25"/>
-      <c r="Y7" s="25"/>
-      <c r="Z7" s="25"/>
-      <c r="AA7" s="25"/>
-      <c r="AB7" s="25"/>
-      <c r="AC7" s="25"/>
-      <c r="AD7" s="23"/>
-      <c r="AE7" s="23"/>
-      <c r="AF7" s="23"/>
-      <c r="AG7" s="23"/>
-      <c r="AH7" s="23"/>
-      <c r="AI7" s="23"/>
-      <c r="AJ7" s="27"/>
+      <c r="R7" s="26"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="26"/>
+      <c r="U7" s="26"/>
+      <c r="V7" s="26"/>
+      <c r="W7" s="26"/>
+      <c r="X7" s="26"/>
+      <c r="Y7" s="26"/>
+      <c r="Z7" s="26"/>
+      <c r="AA7" s="26"/>
+      <c r="AB7" s="26"/>
+      <c r="AC7" s="26"/>
+      <c r="AD7" s="24"/>
+      <c r="AE7" s="24"/>
+      <c r="AF7" s="24"/>
+      <c r="AG7" s="24"/>
+      <c r="AH7" s="24"/>
+      <c r="AI7" s="24"/>
+      <c r="AJ7" s="29"/>
       <c r="AK7" s="20"/>
       <c r="AL7" s="20"/>
       <c r="AM7" s="20"/>
       <c r="AN7" s="20"/>
     </row>
-    <row r="8" spans="1:40" ht="16" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.4">
       <c r="A8" s="21"/>
       <c r="B8" s="22"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
       <c r="J8" s="20"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
       <c r="Q8" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="R8" s="25"/>
-      <c r="S8" s="26"/>
-      <c r="T8" s="25"/>
-      <c r="U8" s="25"/>
-      <c r="V8" s="25"/>
-      <c r="W8" s="25"/>
-      <c r="X8" s="25"/>
-      <c r="Y8" s="25"/>
-      <c r="Z8" s="25"/>
-      <c r="AA8" s="25"/>
-      <c r="AB8" s="25"/>
-      <c r="AC8" s="25"/>
-      <c r="AD8" s="23"/>
-      <c r="AE8" s="23"/>
-      <c r="AF8" s="23"/>
-      <c r="AG8" s="23"/>
-      <c r="AH8" s="23"/>
-      <c r="AI8" s="23"/>
-      <c r="AJ8" s="27"/>
+      <c r="R8" s="26"/>
+      <c r="S8" s="25"/>
+      <c r="T8" s="26"/>
+      <c r="U8" s="26"/>
+      <c r="V8" s="26"/>
+      <c r="W8" s="26"/>
+      <c r="X8" s="26"/>
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="26"/>
+      <c r="AA8" s="26"/>
+      <c r="AB8" s="26"/>
+      <c r="AC8" s="26"/>
+      <c r="AD8" s="24"/>
+      <c r="AE8" s="24"/>
+      <c r="AF8" s="24"/>
+      <c r="AG8" s="24"/>
+      <c r="AH8" s="24"/>
+      <c r="AI8" s="24"/>
+      <c r="AJ8" s="29"/>
       <c r="AK8" s="20"/>
       <c r="AL8" s="20"/>
       <c r="AM8" s="20"/>
       <c r="AN8" s="20"/>
     </row>
-    <row r="9" spans="1:40" ht="16" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.4">
       <c r="A9" s="21"/>
       <c r="B9" s="22"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
       <c r="Q9" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="R9" s="25"/>
-      <c r="S9" s="26"/>
-      <c r="T9" s="25"/>
-      <c r="U9" s="25"/>
-      <c r="V9" s="25"/>
-      <c r="W9" s="25"/>
-      <c r="X9" s="25"/>
-      <c r="Y9" s="25"/>
-      <c r="Z9" s="25"/>
-      <c r="AA9" s="25"/>
-      <c r="AB9" s="25"/>
-      <c r="AC9" s="25"/>
-      <c r="AD9" s="23"/>
-      <c r="AE9" s="23"/>
-      <c r="AF9" s="23"/>
-      <c r="AG9" s="23"/>
-      <c r="AH9" s="23"/>
-      <c r="AI9" s="23"/>
-      <c r="AJ9" s="27"/>
+      <c r="R9" s="26"/>
+      <c r="S9" s="25"/>
+      <c r="T9" s="26"/>
+      <c r="U9" s="26"/>
+      <c r="V9" s="26"/>
+      <c r="W9" s="26"/>
+      <c r="X9" s="26"/>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="26"/>
+      <c r="AA9" s="26"/>
+      <c r="AB9" s="26"/>
+      <c r="AC9" s="26"/>
+      <c r="AD9" s="24"/>
+      <c r="AE9" s="24"/>
+      <c r="AF9" s="24"/>
+      <c r="AG9" s="24"/>
+      <c r="AH9" s="24"/>
+      <c r="AI9" s="24"/>
+      <c r="AJ9" s="29"/>
       <c r="AK9" s="20"/>
       <c r="AL9" s="20"/>
       <c r="AM9" s="20"/>
       <c r="AN9" s="20"/>
     </row>
-    <row r="10" spans="1:40" ht="16" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.4">
       <c r="A10" s="21"/>
       <c r="B10" s="22"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
       <c r="J10" s="20"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
       <c r="Q10" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="R10" s="25"/>
-      <c r="S10" s="26"/>
-      <c r="T10" s="25"/>
-      <c r="U10" s="25"/>
-      <c r="V10" s="25"/>
-      <c r="W10" s="25"/>
-      <c r="X10" s="25"/>
-      <c r="Y10" s="25"/>
-      <c r="Z10" s="25"/>
-      <c r="AA10" s="25"/>
-      <c r="AB10" s="25"/>
-      <c r="AC10" s="25"/>
-      <c r="AD10" s="23"/>
-      <c r="AE10" s="23"/>
-      <c r="AF10" s="23"/>
-      <c r="AG10" s="23"/>
-      <c r="AH10" s="23"/>
-      <c r="AI10" s="23"/>
-      <c r="AJ10" s="27"/>
+      <c r="R10" s="26"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="26"/>
+      <c r="U10" s="26"/>
+      <c r="V10" s="26"/>
+      <c r="W10" s="26"/>
+      <c r="X10" s="26"/>
+      <c r="Y10" s="26"/>
+      <c r="Z10" s="26"/>
+      <c r="AA10" s="26"/>
+      <c r="AB10" s="26"/>
+      <c r="AC10" s="26"/>
+      <c r="AD10" s="24"/>
+      <c r="AE10" s="24"/>
+      <c r="AF10" s="24"/>
+      <c r="AG10" s="24"/>
+      <c r="AH10" s="24"/>
+      <c r="AI10" s="24"/>
+      <c r="AJ10" s="29"/>
       <c r="AK10" s="20"/>
       <c r="AL10" s="20"/>
       <c r="AM10" s="20"/>
       <c r="AN10" s="20"/>
     </row>
-    <row r="11" spans="1:40" ht="16" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.4">
       <c r="A11" s="21"/>
       <c r="B11" s="22"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
       <c r="Q11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="R11" s="25"/>
-      <c r="S11" s="26"/>
-      <c r="T11" s="25"/>
-      <c r="U11" s="25"/>
-      <c r="V11" s="25"/>
-      <c r="W11" s="25"/>
-      <c r="X11" s="25"/>
-      <c r="Y11" s="25"/>
-      <c r="Z11" s="25"/>
-      <c r="AA11" s="25"/>
-      <c r="AB11" s="25"/>
-      <c r="AC11" s="25"/>
-      <c r="AD11" s="23"/>
-      <c r="AE11" s="23"/>
-      <c r="AF11" s="23"/>
-      <c r="AG11" s="23"/>
-      <c r="AH11" s="23"/>
-      <c r="AI11" s="23"/>
-      <c r="AJ11" s="27"/>
+      <c r="R11" s="26"/>
+      <c r="S11" s="25"/>
+      <c r="T11" s="26"/>
+      <c r="U11" s="26"/>
+      <c r="V11" s="26"/>
+      <c r="W11" s="26"/>
+      <c r="X11" s="26"/>
+      <c r="Y11" s="26"/>
+      <c r="Z11" s="26"/>
+      <c r="AA11" s="26"/>
+      <c r="AB11" s="26"/>
+      <c r="AC11" s="26"/>
+      <c r="AD11" s="24"/>
+      <c r="AE11" s="24"/>
+      <c r="AF11" s="24"/>
+      <c r="AG11" s="24"/>
+      <c r="AH11" s="24"/>
+      <c r="AI11" s="24"/>
+      <c r="AJ11" s="29"/>
       <c r="AK11" s="20"/>
       <c r="AL11" s="20"/>
       <c r="AM11" s="20"/>
       <c r="AN11" s="20"/>
     </row>
-    <row r="12" spans="1:40" ht="16" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.4">
       <c r="A12" s="8">
         <v>299</v>
       </c>
@@ -1932,7 +1935,7 @@
         <v>83</v>
       </c>
       <c r="AJ12" s="13"/>
-      <c r="AK12" s="8" t="s">
+      <c r="AK12" s="16" t="s">
         <v>84</v>
       </c>
       <c r="AL12" s="8"/>
@@ -2959,10 +2962,10 @@
       <c r="A26" s="21">
         <v>3473</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="27" t="s">
         <v>189</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="28" t="s">
         <v>189</v>
       </c>
       <c r="D26" s="20"/>
@@ -2984,33 +2987,33 @@
       <c r="J26" s="20">
         <v>1</v>
       </c>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23" t="s">
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="N26" s="23"/>
-      <c r="O26" s="23" t="s">
+      <c r="N26" s="24"/>
+      <c r="O26" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="P26" s="23" t="s">
+      <c r="P26" s="24" t="s">
         <v>193</v>
       </c>
       <c r="Q26" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="R26" s="25"/>
-      <c r="S26" s="25"/>
-      <c r="T26" s="25"/>
-      <c r="U26" s="25"/>
-      <c r="V26" s="25"/>
-      <c r="W26" s="25"/>
-      <c r="X26" s="25"/>
-      <c r="Y26" s="25"/>
-      <c r="Z26" s="25"/>
-      <c r="AA26" s="25"/>
-      <c r="AB26" s="25"/>
-      <c r="AC26" s="25"/>
+      <c r="R26" s="26"/>
+      <c r="S26" s="26"/>
+      <c r="T26" s="26"/>
+      <c r="U26" s="26"/>
+      <c r="V26" s="26"/>
+      <c r="W26" s="26"/>
+      <c r="X26" s="26"/>
+      <c r="Y26" s="26"/>
+      <c r="Z26" s="26"/>
+      <c r="AA26" s="26"/>
+      <c r="AB26" s="26"/>
+      <c r="AC26" s="26"/>
       <c r="AD26" s="20"/>
       <c r="AE26" s="20"/>
       <c r="AF26" s="20"/>
@@ -3025,8 +3028,8 @@
     </row>
     <row r="27" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="21"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="29"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="28"/>
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
@@ -3034,27 +3037,27 @@
       <c r="H27" s="20"/>
       <c r="I27" s="20"/>
       <c r="J27" s="20"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="23"/>
-      <c r="M27" s="23"/>
-      <c r="N27" s="23"/>
-      <c r="O27" s="23"/>
-      <c r="P27" s="23"/>
+      <c r="K27" s="24"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="24"/>
+      <c r="N27" s="24"/>
+      <c r="O27" s="24"/>
+      <c r="P27" s="24"/>
       <c r="Q27" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="R27" s="25"/>
-      <c r="S27" s="25"/>
-      <c r="T27" s="25"/>
-      <c r="U27" s="25"/>
-      <c r="V27" s="25"/>
-      <c r="W27" s="25"/>
-      <c r="X27" s="25"/>
-      <c r="Y27" s="25"/>
-      <c r="Z27" s="25"/>
-      <c r="AA27" s="25"/>
-      <c r="AB27" s="25"/>
-      <c r="AC27" s="25"/>
+      <c r="R27" s="26"/>
+      <c r="S27" s="26"/>
+      <c r="T27" s="26"/>
+      <c r="U27" s="26"/>
+      <c r="V27" s="26"/>
+      <c r="W27" s="26"/>
+      <c r="X27" s="26"/>
+      <c r="Y27" s="26"/>
+      <c r="Z27" s="26"/>
+      <c r="AA27" s="26"/>
+      <c r="AB27" s="26"/>
+      <c r="AC27" s="26"/>
       <c r="AD27" s="20"/>
       <c r="AE27" s="20"/>
       <c r="AF27" s="20"/>
@@ -3069,8 +3072,8 @@
     </row>
     <row r="28" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="21"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="29"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="28"/>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
@@ -3078,27 +3081,27 @@
       <c r="H28" s="20"/>
       <c r="I28" s="20"/>
       <c r="J28" s="20"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="23"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="24"/>
+      <c r="P28" s="24"/>
       <c r="Q28" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="R28" s="25"/>
-      <c r="S28" s="25"/>
-      <c r="T28" s="25"/>
-      <c r="U28" s="25"/>
-      <c r="V28" s="25"/>
-      <c r="W28" s="25"/>
-      <c r="X28" s="25"/>
-      <c r="Y28" s="25"/>
-      <c r="Z28" s="25"/>
-      <c r="AA28" s="25"/>
-      <c r="AB28" s="25"/>
-      <c r="AC28" s="25"/>
+      <c r="R28" s="26"/>
+      <c r="S28" s="26"/>
+      <c r="T28" s="26"/>
+      <c r="U28" s="26"/>
+      <c r="V28" s="26"/>
+      <c r="W28" s="26"/>
+      <c r="X28" s="26"/>
+      <c r="Y28" s="26"/>
+      <c r="Z28" s="26"/>
+      <c r="AA28" s="26"/>
+      <c r="AB28" s="26"/>
+      <c r="AC28" s="26"/>
       <c r="AD28" s="20"/>
       <c r="AE28" s="20"/>
       <c r="AF28" s="20"/>
@@ -3113,8 +3116,8 @@
     </row>
     <row r="29" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="21"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="29"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="28"/>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
@@ -3122,27 +3125,27 @@
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
       <c r="J29" s="20"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="23"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="24"/>
+      <c r="O29" s="24"/>
+      <c r="P29" s="24"/>
       <c r="Q29" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="R29" s="25"/>
-      <c r="S29" s="25"/>
-      <c r="T29" s="25"/>
-      <c r="U29" s="25"/>
-      <c r="V29" s="25"/>
-      <c r="W29" s="25"/>
-      <c r="X29" s="25"/>
-      <c r="Y29" s="25"/>
-      <c r="Z29" s="25"/>
-      <c r="AA29" s="25"/>
-      <c r="AB29" s="25"/>
-      <c r="AC29" s="25"/>
+      <c r="R29" s="26"/>
+      <c r="S29" s="26"/>
+      <c r="T29" s="26"/>
+      <c r="U29" s="26"/>
+      <c r="V29" s="26"/>
+      <c r="W29" s="26"/>
+      <c r="X29" s="26"/>
+      <c r="Y29" s="26"/>
+      <c r="Z29" s="26"/>
+      <c r="AA29" s="26"/>
+      <c r="AB29" s="26"/>
+      <c r="AC29" s="26"/>
       <c r="AD29" s="20"/>
       <c r="AE29" s="20"/>
       <c r="AF29" s="20"/>
@@ -3157,8 +3160,8 @@
     </row>
     <row r="30" spans="1:40" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="21"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="29"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="28"/>
       <c r="D30" s="20"/>
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
@@ -3166,27 +3169,27 @@
       <c r="H30" s="20"/>
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="23"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="23"/>
-      <c r="P30" s="23"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="24"/>
+      <c r="O30" s="24"/>
+      <c r="P30" s="24"/>
       <c r="Q30" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="R30" s="25"/>
-      <c r="S30" s="25"/>
-      <c r="T30" s="25"/>
-      <c r="U30" s="25"/>
-      <c r="V30" s="25"/>
-      <c r="W30" s="25"/>
-      <c r="X30" s="25"/>
-      <c r="Y30" s="25"/>
-      <c r="Z30" s="25"/>
-      <c r="AA30" s="25"/>
-      <c r="AB30" s="25"/>
-      <c r="AC30" s="25"/>
+      <c r="R30" s="26"/>
+      <c r="S30" s="26"/>
+      <c r="T30" s="26"/>
+      <c r="U30" s="26"/>
+      <c r="V30" s="26"/>
+      <c r="W30" s="26"/>
+      <c r="X30" s="26"/>
+      <c r="Y30" s="26"/>
+      <c r="Z30" s="26"/>
+      <c r="AA30" s="26"/>
+      <c r="AB30" s="26"/>
+      <c r="AC30" s="26"/>
       <c r="AD30" s="20"/>
       <c r="AE30" s="20"/>
       <c r="AF30" s="20"/>
@@ -3535,8 +3538,8 @@
       <c r="AM35" s="8"/>
       <c r="AN35" s="8"/>
     </row>
-    <row r="36" spans="1:40" ht="16" x14ac:dyDescent="0.4"/>
   </sheetData>
+  <autoFilter ref="A1:AN35" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="78">
     <mergeCell ref="AM26:AM30"/>
     <mergeCell ref="AN26:AN30"/>
@@ -3546,11 +3549,6 @@
     <mergeCell ref="AJ26:AJ30"/>
     <mergeCell ref="AK26:AK30"/>
     <mergeCell ref="AL26:AL30"/>
-    <mergeCell ref="AA26:AA30"/>
-    <mergeCell ref="AB26:AB30"/>
-    <mergeCell ref="AC26:AC30"/>
-    <mergeCell ref="AD26:AD30"/>
-    <mergeCell ref="AE26:AE30"/>
     <mergeCell ref="AF26:AF30"/>
     <mergeCell ref="U26:U30"/>
     <mergeCell ref="V26:V30"/>
@@ -3558,11 +3556,11 @@
     <mergeCell ref="X26:X30"/>
     <mergeCell ref="Y26:Y30"/>
     <mergeCell ref="Z26:Z30"/>
-    <mergeCell ref="N26:N30"/>
-    <mergeCell ref="O26:O30"/>
-    <mergeCell ref="P26:P30"/>
-    <mergeCell ref="R26:R30"/>
-    <mergeCell ref="S26:S30"/>
+    <mergeCell ref="AA26:AA30"/>
+    <mergeCell ref="AB26:AB30"/>
+    <mergeCell ref="AC26:AC30"/>
+    <mergeCell ref="AD26:AD30"/>
+    <mergeCell ref="AE26:AE30"/>
     <mergeCell ref="T26:T30"/>
     <mergeCell ref="H26:H30"/>
     <mergeCell ref="I26:I30"/>
@@ -3570,6 +3568,11 @@
     <mergeCell ref="K26:K30"/>
     <mergeCell ref="L26:L30"/>
     <mergeCell ref="M26:M30"/>
+    <mergeCell ref="N26:N30"/>
+    <mergeCell ref="O26:O30"/>
+    <mergeCell ref="P26:P30"/>
+    <mergeCell ref="R26:R30"/>
+    <mergeCell ref="S26:S30"/>
     <mergeCell ref="AL2:AL11"/>
     <mergeCell ref="AM2:AM11"/>
     <mergeCell ref="AN2:AN11"/>
@@ -3586,11 +3589,6 @@
     <mergeCell ref="AI2:AI11"/>
     <mergeCell ref="AJ2:AJ11"/>
     <mergeCell ref="AK2:AK11"/>
-    <mergeCell ref="Z2:Z11"/>
-    <mergeCell ref="AA2:AA11"/>
-    <mergeCell ref="AB2:AB11"/>
-    <mergeCell ref="AC2:AC11"/>
-    <mergeCell ref="AD2:AD11"/>
     <mergeCell ref="AE2:AE11"/>
     <mergeCell ref="T2:T11"/>
     <mergeCell ref="U2:U11"/>
@@ -3598,11 +3596,11 @@
     <mergeCell ref="W2:W11"/>
     <mergeCell ref="X2:X11"/>
     <mergeCell ref="Y2:Y11"/>
-    <mergeCell ref="M2:M11"/>
-    <mergeCell ref="N2:N11"/>
-    <mergeCell ref="O2:O11"/>
-    <mergeCell ref="P2:P11"/>
-    <mergeCell ref="R2:R11"/>
+    <mergeCell ref="Z2:Z11"/>
+    <mergeCell ref="AA2:AA11"/>
+    <mergeCell ref="AB2:AB11"/>
+    <mergeCell ref="AC2:AC11"/>
+    <mergeCell ref="AD2:AD11"/>
     <mergeCell ref="S2:S11"/>
     <mergeCell ref="G2:G11"/>
     <mergeCell ref="H2:H11"/>
@@ -3610,16 +3608,22 @@
     <mergeCell ref="J2:J11"/>
     <mergeCell ref="K2:K11"/>
     <mergeCell ref="L2:L11"/>
+    <mergeCell ref="M2:M11"/>
+    <mergeCell ref="N2:N11"/>
+    <mergeCell ref="O2:O11"/>
+    <mergeCell ref="P2:P11"/>
+    <mergeCell ref="R2:R11"/>
+    <mergeCell ref="F2:F11"/>
     <mergeCell ref="A2:A11"/>
     <mergeCell ref="B2:B11"/>
     <mergeCell ref="C2:C11"/>
     <mergeCell ref="D2:D11"/>
     <mergeCell ref="E2:E11"/>
-    <mergeCell ref="F2:F11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AI20" r:id="rId1" xr:uid="{0A1F5157-47BF-473F-8009-72F9AE9BF924}"/>
     <hyperlink ref="AI21" r:id="rId2" xr:uid="{585DAB58-3916-4292-957D-516F2E052B23}"/>
+    <hyperlink ref="AK12" r:id="rId3" xr:uid="{B53CF4F6-CAFE-44C6-A7B6-33CA2DB891C2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>